<commit_message>
Added a welcome window and a selection of products to add
</commit_message>
<xml_diff>
--- a/проект_БД.xlsx
+++ b/проект_БД.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mskou\PycharmProjects\start\Masha\PyQT\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mskou\PycharmProjects\start\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F9C4F0-5142-4B32-92B5-7B16508D2ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51927D22-C1E7-4289-91B8-3ECAA2DD6825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9EDA3A37-562A-42C9-A07C-7F3171B53E5C}"/>
+    <workbookView xWindow="4740" yWindow="600" windowWidth="17280" windowHeight="11640" xr2:uid="{9EDA3A37-562A-42C9-A07C-7F3171B53E5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>время приема</t>
   </si>
   <si>
-    <t>Таблица пользователей</t>
-  </si>
-  <si>
     <t>масса</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Костя</t>
+  </si>
+  <si>
+    <t>Дневник</t>
   </si>
 </sst>
 </file>
@@ -162,19 +162,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -184,6 +178,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -501,7 +498,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,27 +512,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="J1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -556,134 +553,134 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>34</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>14</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>53</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>200</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>100</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>44856</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>1</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="J12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="7" t="s">
+      <c r="J12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O12" s="6"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="4">
+        <v>19</v>
+      </c>
+      <c r="M13" s="3">
         <v>1</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="4"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="4">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3">
         <v>2</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="4"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M15" s="4">
+      <c r="M15" s="3">
         <v>3</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="4"/>
+      <c r="O15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>